<commit_message>
adapted shop and help
</commit_message>
<xml_diff>
--- a/Planning/Planning_9_5_16_5.xlsx
+++ b/Planning/Planning_9_5_16_5.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2614968-EEA5-4690-813F-20D1C694B76D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F979D901-5031-4FCB-8772-F3B15CD09846}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Task</t>
   </si>
@@ -388,16 +388,16 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,7 +417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -428,7 +428,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -439,7 +439,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -450,11 +450,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
       </c>
       <c r="F5" t="s">

</xml_diff>